<commit_message>
Mise à jour des résultats Ajout du package TP
</commit_message>
<xml_diff>
--- a/resultats/tp1/Resultats TP1.xlsx
+++ b/resultats/tp1/Resultats TP1.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12195" windowHeight="4350" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="19470" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Acceuil" sheetId="1" r:id="rId1"/>
     <sheet name="Résultats Gobaux" sheetId="4" r:id="rId2"/>
     <sheet name="1 Serveur" sheetId="3" r:id="rId3"/>
-    <sheet name="4 Serveurs" sheetId="5" r:id="rId4"/>
-    <sheet name="8 Serveurs" sheetId="2" r:id="rId5"/>
-    <sheet name="WorkPlace" sheetId="6" r:id="rId6"/>
+    <sheet name="2 serveurs" sheetId="8" r:id="rId4"/>
+    <sheet name="4 Serveurs" sheetId="5" r:id="rId5"/>
+    <sheet name="6 Serveurs" sheetId="7" r:id="rId6"/>
+    <sheet name="8 Serveurs" sheetId="2" r:id="rId7"/>
+    <sheet name="WorkPlace" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="64">
   <si>
     <t>Exp1</t>
   </si>
@@ -121,10 +123,62 @@
   </si>
   <si>
     <t>Best Results</t>
+  </si>
+  <si>
+    <t>TP1 : Un meilleur résultat avec plus de puissance ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best </t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Mean Score</t>
+  </si>
+  <si>
+    <t>Quartile</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Mediane</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>1 Serveur</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>8 Serveurs</t>
+  </si>
+  <si>
+    <t>Rubrique</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>4 Serveurs</t>
   </si>
   <si>
     <t>Protocole expérimentale :
 Population générée aléatoirement sur un nombre croissant de serveurs disponnibles.
+Une population est générée sur chacun des serveurs
 Le protocole des détails est le suivant :
 &gt; Environement :    berlin52.tsp
 &gt; Taille population :  1000
@@ -137,55 +191,40 @@
 &gt; Condition D'arret Epsilon avec Marge : e=0.01 avec une marge de 100</t>
   </si>
   <si>
-    <t>TP1 : Un meilleur résultat avec plus de puissance ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best </t>
-  </si>
-  <si>
-    <t>Temps</t>
-  </si>
-  <si>
-    <t>Best</t>
-  </si>
-  <si>
-    <t>Mean Score</t>
-  </si>
-  <si>
-    <t>Quartile</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Mediane</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>1 Serveur</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Med</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>8 Serveurs</t>
-  </si>
-  <si>
-    <t>Rubrique</t>
-  </si>
-  <si>
-    <t>Moyenne</t>
-  </si>
-  <si>
-    <t>4 Serveurs</t>
+    <t>Exp11</t>
+  </si>
+  <si>
+    <t>Exp12</t>
+  </si>
+  <si>
+    <t>Exp13</t>
+  </si>
+  <si>
+    <t>Exp14</t>
+  </si>
+  <si>
+    <t>Exp15</t>
+  </si>
+  <si>
+    <t>Exp16</t>
+  </si>
+  <si>
+    <t>Exp17</t>
+  </si>
+  <si>
+    <t>Exp18</t>
+  </si>
+  <si>
+    <t>Exp19</t>
+  </si>
+  <si>
+    <t>Exp20</t>
+  </si>
+  <si>
+    <t>2 Serveur</t>
+  </si>
+  <si>
+    <t>6 Serveurs</t>
   </si>
 </sst>
 </file>
@@ -534,16 +573,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Résultats Gobaux'!$C$2:$E$2</c:f>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1 Serveur</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4 Serveurs</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8 Serveurs</c:v>
                 </c:pt>
               </c:strCache>
@@ -551,14 +596,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Résultats Gobaux'!$C$4:$E$4</c:f>
+              <c:f>'Résultats Gobaux'!$C$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16812.26592596815</c:v>
+                  <c:v>16794.270831893176</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15917.372799859175</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15946.072727105726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15427.195348363324</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>15249.4333407834</c:v>
                 </c:pt>
               </c:numCache>
@@ -598,16 +652,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Résultats Gobaux'!$C$2:$E$2</c:f>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1 Serveur</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4 Serveurs</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8 Serveurs</c:v>
                 </c:pt>
               </c:strCache>
@@ -615,14 +675,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Résultats Gobaux'!$C$3:$E$3</c:f>
+              <c:f>'Résultats Gobaux'!$C$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15709.493106382401</c:v>
+                  <c:v>15531.6099919236</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14795.501080481799</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15317.8296075493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15008.8221828638</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>14792.957531804201</c:v>
                 </c:pt>
               </c:numCache>
@@ -660,16 +729,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Résultats Gobaux'!$C$2:$E$2</c:f>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1 Serveur</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4 Serveurs</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8 Serveurs</c:v>
                 </c:pt>
               </c:strCache>
@@ -677,15 +752,117 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Résultats Gobaux'!$C$5:$E$5</c:f>
+              <c:f>'Résultats Gobaux'!$C$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18450.222206240702</c:v>
+                  <c:v>17891.90830360715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16364.3370863543</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>16207.808734852</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15522.952849192399</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>15524.656451826999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Résultats Gobaux'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Moyenne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.22383026073836579"/>
+                  <c:y val="0.2931003605785294"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8 Serveurs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Résultats Gobaux'!$C$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17965.608830982193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16512.102140909388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16391.579113758617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16008.894324894491</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15976.228641433088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,7 +871,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>'Résultats Gobaux'!$B$7</c:f>
@@ -724,16 +901,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Résultats Gobaux'!$C$2:$E$2</c:f>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1 Serveur</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4 Serveurs</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8 Serveurs</c:v>
                 </c:pt>
               </c:strCache>
@@ -741,14 +924,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Résultats Gobaux'!$C$7:$E$7</c:f>
+              <c:f>'Résultats Gobaux'!$C$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>21390.963973779501</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>18206.427376312899</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>21390.963973779501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17971.726583877498</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>17663.323202329299</c:v>
                 </c:pt>
               </c:numCache>
@@ -758,7 +950,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>'Résultats Gobaux'!$B$6</c:f>
@@ -780,16 +972,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Résultats Gobaux'!$C$2:$E$2</c:f>
+              <c:f>'Résultats Gobaux'!$C$2:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1 Serveur</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2 Serveur</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4 Serveurs</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>6 Serveurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8 Serveurs</c:v>
                 </c:pt>
               </c:strCache>
@@ -797,14 +995,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Résultats Gobaux'!$C$6:$E$6</c:f>
+              <c:f>'Résultats Gobaux'!$C$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19588.933807831898</c:v>
+                  <c:v>19023.666348511077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17524.609520766448</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>16838.016342181323</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16567.452842813473</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16909.337175456774</c:v>
                 </c:pt>
               </c:numCache>
@@ -830,7 +1037,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:upDownBars>
-          <c:gapWidth val="150"/>
+          <c:gapWidth val="500"/>
           <c:upBars>
             <c:spPr>
               <a:gradFill>
@@ -874,11 +1081,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44173312"/>
-        <c:axId val="621610688"/>
+        <c:axId val="578976768"/>
+        <c:axId val="577029248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44173312"/>
+        <c:axId val="578976768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +1095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="621610688"/>
+        <c:crossAx val="577029248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -897,7 +1104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="621610688"/>
+        <c:axId val="577029248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10000"/>
@@ -909,7 +1116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44173312"/>
+        <c:crossAx val="578976768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,9 +1177,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'1 Serveur'!$B$2:$B$12</c:f>
+              <c:f>'1 Serveur'!$B$2:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Experience</c:v>
                 </c:pt>
@@ -1005,16 +1212,46 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Exp10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Exp11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Exp12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Exp13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Exp14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Exp15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Exp16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Exp17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Exp18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Exp19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Exp20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 Serveur'!$C$2:$C$12</c:f>
+              <c:f>'1 Serveur'!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1047,6 +1284,36 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>19748.9508255728</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16574.859402352798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18288.777294370499</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16867.4079750733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17023.4407807262</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17616.424881638999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19451.211567993301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16981.1000668579</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15531.6099919236</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18817.237729883698</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17994.807640667699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,11 +1328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44459008"/>
-        <c:axId val="635194752"/>
+        <c:axId val="581538304"/>
+        <c:axId val="577032128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44459008"/>
+        <c:axId val="581538304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635194752"/>
+        <c:crossAx val="577032128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1082,7 +1349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="635194752"/>
+        <c:axId val="577032128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44459008"/>
+        <c:crossAx val="581538304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1129,10 +1396,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1143,51 +1406,40 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1 Serveur'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'1 Serveur'!$B$2:$B$12</c:f>
+              <c:f>'2 serveurs'!$B$3:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Experience</c:v>
+                  <c:v>Exp1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Exp1</c:v>
+                  <c:v>Exp2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Exp2</c:v>
+                  <c:v>Exp3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Exp3</c:v>
+                  <c:v>Exp4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Exp4</c:v>
+                  <c:v>Exp5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Exp5</c:v>
+                  <c:v>Exp6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Exp6</c:v>
+                  <c:v>Exp7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Exp7</c:v>
+                  <c:v>Exp8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Exp8</c:v>
+                  <c:v>Exp9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Exp9</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>Exp10</c:v>
                 </c:pt>
               </c:strCache>
@@ -1195,42 +1447,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 Serveur'!$C$2:$C$12</c:f>
+              <c:f>'2 serveurs'!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>18206.427376312899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16353.6739758489</c:v>
+                  <c:v>16422.1666724604</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21390.963973779501</c:v>
+                  <c:v>18045.924375663399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18995.2608798117</c:v>
+                  <c:v>16306.507500248201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15709.493106382401</c:v>
+                  <c:v>17779.808339852199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17905.1835326697</c:v>
+                  <c:v>16150.293084630801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17878.633074544599</c:v>
+                  <c:v>15839.732704935301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16456.810209775998</c:v>
+                  <c:v>14795.501080481799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20617.4469551611</c:v>
+                  <c:v>16759.013063509199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19108.8827546092</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>19748.9508255728</c:v>
+                  <c:v>14815.647210999699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1245,11 +1494,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44531200"/>
-        <c:axId val="43748736"/>
+        <c:axId val="567635968"/>
+        <c:axId val="577034432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44531200"/>
+        <c:axId val="567635968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43748736"/>
+        <c:crossAx val="577034432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1266,7 +1515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43748736"/>
+        <c:axId val="577034432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,14 +1526,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44531200"/>
+        <c:crossAx val="567635968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1319,7 +1567,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12812729658792651"/>
+          <c:y val="0.1901738845144357"/>
+          <c:w val="0.65508202099737534"/>
+          <c:h val="0.62520195392242639"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1329,7 +1587,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8 Serveurs'!$H$3</c:f>
+              <c:f>'4 Serveurs'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1341,7 +1599,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'8 Serveurs'!$G$4:$G$13</c:f>
+              <c:f>'4 Serveurs'!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1379,39 +1637,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8 Serveurs'!$H$4:$H$13</c:f>
+              <c:f>'4 Serveurs'!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>16234.0854205546</c:v>
+                  <c:v>16465.561322538801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15637.599306330199</c:v>
+                  <c:v>16182.8851722288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15333.156881459399</c:v>
+                  <c:v>15848.559988937401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17425.7875045941</c:v>
+                  <c:v>16001.950970345501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14792.957531804201</c:v>
+                  <c:v>15927.446646025801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17134.421093757501</c:v>
+                  <c:v>17244.480566350499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14907.7163822864</c:v>
+                  <c:v>16232.732297475201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15411.7135973238</c:v>
+                  <c:v>16962.168015395499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17663.323202329299</c:v>
+                  <c:v>15317.8296075493</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15221.5254938914</c:v>
+                  <c:v>17732.176550739401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,11 +1684,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44461568"/>
-        <c:axId val="635197632"/>
+        <c:axId val="567638016"/>
+        <c:axId val="581100096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44461568"/>
+        <c:axId val="567638016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,7 +1697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="635197632"/>
+        <c:crossAx val="581100096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1447,7 +1705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="635197632"/>
+        <c:axId val="581100096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,7 +1716,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44461568"/>
+        <c:crossAx val="567638016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,20 +1738,380 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'6 Serveurs'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Results</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'6 Serveurs'!$B$4:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Exp1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Exp2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Exp3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Exp4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Exp5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Exp6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exp7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Exp8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Exp9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Exp10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'6 Serveurs'!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>16602.881837193199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16903.0487569336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15426.1442744245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17971.726583877498</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15598.5229473789</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16461.1658596743</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15008.8221828638</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15447.3827510059</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15238.8994854134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15430.3485701798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="74065408"/>
+        <c:axId val="57181888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="74065408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57181888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="57181888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74065408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'8 Serveurs'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Results</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'8 Serveurs'!$G$4:$G$13</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Exp1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Exp2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Exp3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Exp4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Exp5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Exp6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exp7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Exp8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Exp9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Exp10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8 Serveurs'!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>16234.0854205546</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15637.599306330199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15333.156881459399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17425.7875045941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14792.957531804201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17134.421093757501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14907.7163822864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15411.7135973238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17663.323202329299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15221.5254938914</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="578543616"/>
+        <c:axId val="581102976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="578543616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="581102976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="581102976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="578543616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>290512</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1554,23 +2172,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1588,6 +2204,76 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1623,12 +2309,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B2:E8" totalsRowShown="0">
-  <autoFilter ref="B2:E8"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B2:G8" totalsRowShown="0">
+  <autoFilter ref="B2:G8"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Rubrique"/>
     <tableColumn id="2" name="1 Serveur"/>
+    <tableColumn id="5" name="2 Serveur"/>
     <tableColumn id="4" name="4 Serveurs"/>
+    <tableColumn id="6" name="6 Serveurs"/>
     <tableColumn id="3" name="8 Serveurs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1636,7 +2324,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau37" displayName="Tableau37" ref="B2:E12" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau37" displayName="Tableau37" ref="B2:E22" totalsRowShown="0">
+  <autoFilter ref="B2:E22"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Experience"/>
+    <tableColumn id="2" name="Best Results"/>
+    <tableColumn id="3" name="Mean Of Results"/>
+    <tableColumn id="4" name="Mean Time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau37220" displayName="Tableau37220" ref="B2:E12" totalsRowShown="0">
   <autoFilter ref="B2:E12"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Experience"/>
@@ -1648,9 +2349,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau372" displayName="Tableau372" ref="B15:E25" totalsRowShown="0">
-  <autoFilter ref="B15:E25"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau372" displayName="Tableau372" ref="B2:E12" totalsRowShown="0">
+  <autoFilter ref="B2:E12"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Experience"/>
     <tableColumn id="2" name="Best Results"/>
@@ -1661,7 +2362,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau378" displayName="Tableau378" ref="B3:E13" totalsRowShown="0">
+  <autoFilter ref="B3:E13"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Experience"/>
+    <tableColumn id="2" name="Best Results"/>
+    <tableColumn id="3" name="Mean Of Results"/>
+    <tableColumn id="4" name="Mean Time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B3:E84" totalsRowShown="0">
   <autoFilter ref="B3:E84"/>
   <tableColumns count="4">
@@ -1674,7 +2388,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="G3:J13" totalsRowShown="0">
   <autoFilter ref="G3:J13"/>
   <tableColumns count="4">
@@ -1691,9 +2405,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:C4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="B3:C4"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:C11" totalsRowShown="0">
+  <autoFilter ref="B3:C11"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Score"/>
     <tableColumn id="2" name="Temps"/>
@@ -1995,7 +2709,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2720,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2021,7 +2735,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -2257,107 +2971,186 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <f>QUARTILE(Tableau37[Best Results],0)</f>
-        <v>15709.493106382401</v>
+        <v>15531.6099919236</v>
+      </c>
+      <c r="D3">
+        <f>QUARTILE(Tableau37220[Best Results],0)</f>
+        <v>14795.501080481799</v>
       </c>
       <c r="E3">
+        <f>QUARTILE(Tableau372[Best Results],0)</f>
+        <v>15317.8296075493</v>
+      </c>
+      <c r="F3">
+        <f>QUARTILE(Tableau378[Best Results],0)</f>
+        <v>15008.8221828638</v>
+      </c>
+      <c r="G3">
         <f>QUARTILE(Tableau5[Best Results],0)</f>
         <v>14792.957531804201</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <f>QUARTILE(Tableau37[Best Results],1)</f>
-        <v>16812.26592596815</v>
+        <v>16794.270831893176</v>
+      </c>
+      <c r="D4">
+        <f>QUARTILE(Tableau37220[Best Results],1)</f>
+        <v>15917.372799859175</v>
       </c>
       <c r="E4">
+        <f>QUARTILE(Tableau372[Best Results],1)</f>
+        <v>15946.072727105726</v>
+      </c>
+      <c r="F4">
+        <f>QUARTILE(Tableau378[Best Results],1)</f>
+        <v>15427.195348363324</v>
+      </c>
+      <c r="G4">
         <f>QUARTILE(Tableau5[Best Results],1)</f>
         <v>15249.4333407834</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <f>QUARTILE(Tableau37[Best Results],2)</f>
-        <v>18450.222206240702</v>
+        <v>17891.90830360715</v>
+      </c>
+      <c r="D5">
+        <f>QUARTILE(Tableau37220[Best Results],2)</f>
+        <v>16364.3370863543</v>
       </c>
       <c r="E5">
+        <f>QUARTILE(Tableau372[Best Results],2)</f>
+        <v>16207.808734852</v>
+      </c>
+      <c r="F5">
+        <f>QUARTILE(Tableau378[Best Results],2)</f>
+        <v>15522.952849192399</v>
+      </c>
+      <c r="G5">
         <f>QUARTILE(Tableau5[Best Results],2)</f>
         <v>15524.656451826999</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <f>QUARTILE(Tableau37[Best Results],3)</f>
-        <v>19588.933807831898</v>
+        <v>19023.666348511077</v>
+      </c>
+      <c r="D6">
+        <f>QUARTILE(Tableau37220[Best Results],3)</f>
+        <v>17524.609520766448</v>
       </c>
       <c r="E6">
+        <f>QUARTILE(Tableau372[Best Results],3)</f>
+        <v>16838.016342181323</v>
+      </c>
+      <c r="F6">
+        <f>QUARTILE(Tableau378[Best Results],3)</f>
+        <v>16567.452842813473</v>
+      </c>
+      <c r="G6">
         <f>QUARTILE(Tableau5[Best Results],3)</f>
         <v>16909.337175456774</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <f>QUARTILE(Tableau37[Best Results],4)</f>
         <v>21390.963973779501</v>
       </c>
+      <c r="D7">
+        <f>QUARTILE(Tableau37220[Best Results],4)</f>
+        <v>18206.427376312899</v>
+      </c>
       <c r="E7">
+        <f>QUARTILE(Tableau37[Best Results],4)</f>
+        <v>21390.963973779501</v>
+      </c>
+      <c r="F7">
+        <f>QUARTILE(Tableau378[Best Results],4)</f>
+        <v>17971.726583877498</v>
+      </c>
+      <c r="G7">
         <f>QUARTILE(Tableau5[Best Results],4)</f>
         <v>17663.323202329299</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <f>AVERAGE(Tableau37[Best Results])</f>
-        <v>18416.529928815587</v>
+        <v>17965.608830982193</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(Tableau37220[Best Results])</f>
+        <v>16512.102140909388</v>
       </c>
       <c r="E8">
+        <f>AVERAGE(Tableau372[Best Results])</f>
+        <v>16391.579113758617</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(Tableau378[Best Results])</f>
+        <v>16008.894324894491</v>
+      </c>
+      <c r="G8">
         <f>SUM(Tableau5[Best Results])/10</f>
         <v>15976.228641433088</v>
       </c>
@@ -2373,10 +3166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E28"/>
+  <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,6 +3335,777 @@
         <v>64109</v>
       </c>
     </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>16574.859402352798</v>
+      </c>
+      <c r="D13">
+        <v>16574.859402352798</v>
+      </c>
+      <c r="E13">
+        <v>179715</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <v>18288.777294370499</v>
+      </c>
+      <c r="D14">
+        <v>18288.777294370499</v>
+      </c>
+      <c r="E14">
+        <v>90635</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>16867.4079750733</v>
+      </c>
+      <c r="D15">
+        <v>16867.4079750733</v>
+      </c>
+      <c r="E15">
+        <v>98882</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>17023.4407807262</v>
+      </c>
+      <c r="D16">
+        <v>17023.4407807262</v>
+      </c>
+      <c r="E16">
+        <v>195452</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>17616.424881638999</v>
+      </c>
+      <c r="D17">
+        <v>17616.424881638999</v>
+      </c>
+      <c r="E17">
+        <v>116931</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18">
+        <v>19451.211567993301</v>
+      </c>
+      <c r="D18">
+        <v>19451.211567993301</v>
+      </c>
+      <c r="E18">
+        <v>140115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19">
+        <v>16981.1000668579</v>
+      </c>
+      <c r="D19">
+        <v>16981.1000668579</v>
+      </c>
+      <c r="E19">
+        <v>197452</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20">
+        <v>15531.6099919236</v>
+      </c>
+      <c r="D20">
+        <v>15531.6099919236</v>
+      </c>
+      <c r="E20">
+        <v>79872</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <v>18817.237729883698</v>
+      </c>
+      <c r="D21">
+        <v>18817.237729883698</v>
+      </c>
+      <c r="E21">
+        <v>128870</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>17994.807640667699</v>
+      </c>
+      <c r="D22">
+        <v>17994.807640667699</v>
+      </c>
+      <c r="E22">
+        <v>64109</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22">
+        <f>MIN(Tableau37[Best Results])</f>
+        <v>15531.6099919236</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23">
+        <f>MAX(Tableau37[Best Results])</f>
+        <v>21390.963973779501</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25">
+        <f>AVERAGE(Tableau37[Best Results])</f>
+        <v>17965.608830982193</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26">
+        <f>AVERAGE(Tableau37[Mean Of Results])</f>
+        <v>17965.608830982193</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27">
+        <f>SUM(Tableau37[Mean Time])/10</f>
+        <v>258406.6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="18">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J29">
+        <f>QUARTILE(Tableau37[Best Results],0)</f>
+        <v>15531.6099919236</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="18">
+        <v>1</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30">
+        <f>QUARTILE(Tableau37[Best Results],1)</f>
+        <v>16794.270831893176</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="18">
+        <v>2</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31">
+        <f>QUARTILE(Tableau37[Best Results],2)</f>
+        <v>17891.90830360715</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="18">
+        <v>3</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32">
+        <f>QUARTILE(Tableau37[Best Results],3)</f>
+        <v>19023.666348511077</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="18">
+        <v>4</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33">
+        <f>QUARTILE(Tableau37[Best Results],4)</f>
+        <v>21390.963973779501</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H20:J20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I26"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>18206.427376312899</v>
+      </c>
+      <c r="D3">
+        <v>18327.06779957495</v>
+      </c>
+      <c r="E3">
+        <v>557008</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>16422.1666724604</v>
+      </c>
+      <c r="D4">
+        <v>17801.105304198201</v>
+      </c>
+      <c r="E4">
+        <v>723807</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>18045.924375663399</v>
+      </c>
+      <c r="D5">
+        <v>18312.218048740149</v>
+      </c>
+      <c r="E5">
+        <v>562261</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>16306.507500248201</v>
+      </c>
+      <c r="D6">
+        <v>17444.679925959048</v>
+      </c>
+      <c r="E6">
+        <v>564085</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>17779.808339852199</v>
+      </c>
+      <c r="D7">
+        <v>17950.732320548101</v>
+      </c>
+      <c r="E7">
+        <v>727559</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>16150.293084630801</v>
+      </c>
+      <c r="D8">
+        <v>16520.926715443351</v>
+      </c>
+      <c r="E8">
+        <v>527140</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>15839.732704935301</v>
+      </c>
+      <c r="D9">
+        <v>16683.097301121699</v>
+      </c>
+      <c r="E9">
+        <v>771900</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>14795.501080481799</v>
+      </c>
+      <c r="D10">
+        <v>15713.57327180255</v>
+      </c>
+      <c r="E10">
+        <v>662671</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>16759.013063509199</v>
+      </c>
+      <c r="D11">
+        <v>17603.834953003352</v>
+      </c>
+      <c r="E11">
+        <v>660049</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>14815.647210999699</v>
+      </c>
+      <c r="D12">
+        <v>15336.91713199735</v>
+      </c>
+      <c r="E12">
+        <v>996907</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15">
+        <f>MIN(Tableau37220[Best Results])</f>
+        <v>14795.501080481799</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16">
+        <f>MAX(Tableau37220[Best Results])</f>
+        <v>18206.427376312899</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18">
+        <f>AVERAGE(Tableau37220[Best Results])</f>
+        <v>16512.102140909388</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19">
+        <f>AVERAGE(Tableau37220[Mean Of Results])</f>
+        <v>17169.415277238877</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20">
+        <f>SUM(Tableau37220[Mean Time])/10</f>
+        <v>675338.7</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22">
+        <f>QUARTILE(Tableau37220[Best Results],0)</f>
+        <v>14795.501080481799</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="18">
+        <v>1</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23">
+        <f>QUARTILE(Tableau37220[Best Results],1)</f>
+        <v>15917.372799859175</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="18">
+        <v>2</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24">
+        <f>QUARTILE(Tableau37220[Best Results],2)</f>
+        <v>16364.3370863543</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="18">
+        <v>3</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25">
+        <f>QUARTILE(Tableau37220[Best Results],3)</f>
+        <v>17524.609520766448</v>
+      </c>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="18">
+        <v>4</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26">
+        <f>QUARTILE(Tableau37220[Best Results],4)</f>
+        <v>18206.427376312899</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G13:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>16465.561322538801</v>
+      </c>
+      <c r="D3">
+        <v>17410.908583658747</v>
+      </c>
+      <c r="E3">
+        <v>125437.75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>16182.8851722288</v>
+      </c>
+      <c r="D4">
+        <v>17579.189284909025</v>
+      </c>
+      <c r="E4">
+        <v>92433.75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>15848.559988937401</v>
+      </c>
+      <c r="D5">
+        <v>16901.433990236448</v>
+      </c>
+      <c r="E5">
+        <v>120412.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>16001.950970345501</v>
+      </c>
+      <c r="D6">
+        <v>17006.907877541049</v>
+      </c>
+      <c r="E6">
+        <v>116374</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>15927.446646025801</v>
+      </c>
+      <c r="D7">
+        <v>16416.936037511499</v>
+      </c>
+      <c r="E7">
+        <v>126549</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>17244.480566350499</v>
+      </c>
+      <c r="D8">
+        <v>18395.837093551949</v>
+      </c>
+      <c r="E8">
+        <v>94849.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>16232.732297475201</v>
+      </c>
+      <c r="D9">
+        <v>17154.469902495275</v>
+      </c>
+      <c r="E9">
+        <v>113256.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>16962.168015395499</v>
+      </c>
+      <c r="D10">
+        <v>17633.123622292776</v>
+      </c>
+      <c r="E10">
+        <v>111840.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>15317.8296075493</v>
+      </c>
+      <c r="D11">
+        <v>17573.529298558824</v>
+      </c>
+      <c r="E11">
+        <v>105692.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>17732.176550739401</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(Tableau2[Score])</f>
+        <v>18746.474153893385</v>
+      </c>
+      <c r="E12">
+        <v>88895.75</v>
+      </c>
+    </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>30</v>
@@ -2561,8 +4125,8 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17">
-        <f>MIN(Tableau37[Best Results])</f>
-        <v>15709.493106382401</v>
+        <f>MIN(Tableau372[Best Results])</f>
+        <v>15317.8296075493</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -2571,8 +4135,8 @@
       </c>
       <c r="C18" s="18"/>
       <c r="D18">
-        <f>MAX(Tableau37[Best Results])</f>
-        <v>21390.963973779501</v>
+        <f>MAX(Tableau372[Best Results])</f>
+        <v>17732.176550739401</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -2583,12 +4147,12 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20">
-        <f>AVERAGE(Tableau37[Best Results])</f>
-        <v>18416.529928815587</v>
+        <f>AVERAGE(Tableau372[Best Results])</f>
+        <v>16391.579113758617</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -2597,8 +4161,8 @@
       </c>
       <c r="C21" s="18"/>
       <c r="D21">
-        <f>AVERAGE(Tableau37[Mean Of Results])</f>
-        <v>18416.529928815587</v>
+        <f>AVERAGE(Tableau372[Mean Of Results])</f>
+        <v>17481.8809844649</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -2607,13 +4171,13 @@
       </c>
       <c r="C22" s="18"/>
       <c r="D22">
-        <f>SUM(Tableau37[Mean Time])/10</f>
-        <v>129203.3</v>
+        <f>SUM(Tableau372[Mean Time])/10</f>
+        <v>109574.175</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="17"/>
     </row>
@@ -2622,11 +4186,11 @@
         <v>0</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24">
-        <f>QUARTILE(Tableau37[Best Results],0)</f>
-        <v>15709.493106382401</v>
+        <f>QUARTILE(Tableau372[Best Results],0)</f>
+        <v>15317.8296075493</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -2634,11 +4198,11 @@
         <v>1</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25">
-        <f>QUARTILE(Tableau37[Best Results],1)</f>
-        <v>16812.26592596815</v>
+        <f>QUARTILE(Tableau372[Best Results],1)</f>
+        <v>15946.072727105726</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2646,11 +4210,11 @@
         <v>2</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26">
-        <f>QUARTILE(Tableau37[Best Results],2)</f>
-        <v>18450.222206240702</v>
+        <f>QUARTILE(Tableau372[Best Results],2)</f>
+        <v>16207.808734852</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2658,11 +4222,11 @@
         <v>3</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27">
-        <f>QUARTILE(Tableau37[Best Results],3)</f>
-        <v>19588.933807831898</v>
+        <f>QUARTILE(Tableau372[Best Results],3)</f>
+        <v>16838.016342181323</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -2670,7 +4234,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <f>QUARTILE(Tableau37[Best Results],4)</f>
@@ -2689,314 +4253,359 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B15:E41"/>
+  <dimension ref="B3:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:D41"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>16602.881837193199</v>
+      </c>
+      <c r="D4">
+        <v>17477.583795831015</v>
+      </c>
+      <c r="E4">
+        <v>682403</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>16903.0487569336</v>
+      </c>
+      <c r="D5">
+        <v>17930.047347968299</v>
+      </c>
+      <c r="E5">
+        <v>687067</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>15426.1442744245</v>
+      </c>
+      <c r="D6">
+        <v>17846.213869560965</v>
+      </c>
+      <c r="E6">
+        <v>693727</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>17971.726583877498</v>
+      </c>
+      <c r="D7">
+        <v>18571.580839888382</v>
+      </c>
+      <c r="E7">
+        <v>687637</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>15598.5229473789</v>
+      </c>
+      <c r="D8">
+        <v>18209.775745722483</v>
+      </c>
+      <c r="E8">
+        <v>623917</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>16461.1658596743</v>
+      </c>
+      <c r="D9">
+        <v>17329.757968376449</v>
+      </c>
+      <c r="E9">
+        <v>771011</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>15008.8221828638</v>
+      </c>
+      <c r="D10">
+        <v>17286.206647283634</v>
+      </c>
+      <c r="E10">
+        <v>731770</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>15447.3827510059</v>
+      </c>
+      <c r="D11">
+        <v>16770.728817777333</v>
+      </c>
+      <c r="E11">
+        <v>715915</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>15238.8994854134</v>
+      </c>
+      <c r="D12">
+        <v>17471.2539212378</v>
+      </c>
+      <c r="E12">
+        <v>671024</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>15430.3485701798</v>
+      </c>
+      <c r="D13">
+        <v>18746.474153893385</v>
+      </c>
+      <c r="E13">
+        <v>627586</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23">
+        <f>MIN(Tableau378[Best Results])</f>
+        <v>15008.8221828638</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24">
+        <f>MAX(Tableau378[Best Results])</f>
+        <v>17971.726583877498</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26">
+        <f>AVERAGE(Tableau378[Best Results])</f>
+        <v>16008.894324894491</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27">
+        <f>AVERAGE(Tableau378[Mean Of Results])</f>
+        <v>17763.962310753974</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28">
+        <f>SUM(Tableau378[Mean Time])/10</f>
+        <v>689205.7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="18">
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>16353.6739758489</v>
-      </c>
-      <c r="D16">
-        <v>16353.6739758489</v>
-      </c>
-      <c r="E16">
-        <v>179715</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
-        <v>21390.963973779501</v>
-      </c>
-      <c r="D17">
-        <v>21390.963973779501</v>
-      </c>
-      <c r="E17">
-        <v>90635</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>18995.2608798117</v>
-      </c>
-      <c r="D18">
-        <v>18995.2608798117</v>
-      </c>
-      <c r="E18">
-        <v>98882</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
-        <v>15709.493106382401</v>
-      </c>
-      <c r="D19">
-        <v>15709.493106382401</v>
-      </c>
-      <c r="E19">
-        <v>195452</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>17905.1835326697</v>
-      </c>
-      <c r="D20">
-        <v>17905.1835326697</v>
-      </c>
-      <c r="E20">
-        <v>116931</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>17878.633074544599</v>
-      </c>
-      <c r="D21">
-        <v>17878.633074544599</v>
-      </c>
-      <c r="E21">
-        <v>140115</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22">
-        <v>16456.810209775998</v>
-      </c>
-      <c r="D22">
-        <v>16456.810209775998</v>
-      </c>
-      <c r="E22">
-        <v>197452</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23">
-        <v>20617.4469551611</v>
-      </c>
-      <c r="D23">
-        <v>20617.4469551611</v>
-      </c>
-      <c r="E23">
-        <v>79872</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>19108.8827546092</v>
-      </c>
-      <c r="D24">
-        <v>19108.8827546092</v>
-      </c>
-      <c r="E24">
-        <v>128870</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25">
-        <v>19748.9508255728</v>
-      </c>
-      <c r="D25">
-        <v>19748.9508255728</v>
-      </c>
-      <c r="E25">
-        <v>64109</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30">
-        <f>MIN(Tableau372[Best Results])</f>
-        <v>15709.493106382401</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31">
-        <f>MAX(Tableau372[Best Results])</f>
-        <v>21390.963973779501</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33">
-        <f>AVERAGE(Tableau372[Best Results])</f>
-        <v>18416.529928815587</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34">
-        <f>AVERAGE(Tableau372[Mean Of Results])</f>
-        <v>18416.529928815587</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35">
-        <f>SUM(Tableau372[Mean Time])/10</f>
-        <v>129203.3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="s">
+      <c r="I30" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="18">
-        <v>0</v>
-      </c>
-      <c r="C37" s="18" t="s">
+      <c r="J30">
+        <f>QUARTILE(Tableau378[Best Results],0)</f>
+        <v>15008.8221828638</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="18">
+        <v>1</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31">
+        <f>QUARTILE(Tableau378[Best Results],1)</f>
+        <v>15427.195348363324</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="18">
+        <v>2</v>
+      </c>
+      <c r="I32" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D37">
-        <f>QUARTILE(Tableau37[Best Results],0)</f>
-        <v>15709.493106382401</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="18">
-        <v>1</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38">
-        <f>QUARTILE(Tableau37[Best Results],1)</f>
-        <v>16812.26592596815</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="18">
-        <v>2</v>
-      </c>
-      <c r="C39" s="18" t="s">
+      <c r="J32">
+        <f>QUARTILE(Tableau378[Best Results],2)</f>
+        <v>15522.952849192399</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="18">
+        <v>3</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33">
+        <f>QUARTILE(Tableau378[Best Results],3)</f>
+        <v>16567.452842813473</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="18">
+        <v>4</v>
+      </c>
+      <c r="I34" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D39">
-        <f>QUARTILE(Tableau37[Best Results],2)</f>
-        <v>18450.222206240702</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="18">
-        <v>3</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40">
-        <f>QUARTILE(Tableau37[Best Results],3)</f>
-        <v>19588.933807831898</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="18">
-        <v>4</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41">
-        <f>QUARTILE(Tableau37[Best Results],4)</f>
-        <v>21390.963973779501</v>
+      <c r="J34">
+        <f>QUARTILE(Tableau378[Best Results],4)</f>
+        <v>17971.726583877498</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="H21:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3006,12 +4615,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J84"/>
   <sheetViews>
-    <sheetView topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,8 +5031,8 @@
       </c>
       <c r="H18" s="18"/>
       <c r="I18">
-        <f>MAX(Tableau4[Score])</f>
-        <v>20389.2875926909</v>
+        <f>MAX(Tableau5[Best Results])</f>
+        <v>17663.323202329299</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -3449,7 +5058,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="4"/>
       <c r="G20" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20">
@@ -3515,7 +5124,7 @@
         <v>96605</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="17"/>
     </row>
@@ -3536,7 +5145,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24">
         <f>QUARTILE(Tableau5[Best Results],0)</f>
@@ -3560,7 +5169,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25">
         <f>QUARTILE(Tableau5[Best Results],1)</f>
@@ -3584,7 +5193,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I26">
         <f>QUARTILE(Tableau5[Best Results],2)</f>
@@ -3608,7 +5217,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I27">
         <f>QUARTILE(Tableau5[Best Results],3)</f>
@@ -3632,7 +5241,7 @@
         <v>4</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28">
         <f>QUARTILE(Tableau5[Best Results],4)</f>
@@ -4437,15 +6046,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B3:F6"/>
+  <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F4" sqref="F4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,39 +6062,81 @@
     <col min="2" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="G3" t="s">
         <v>38</v>
       </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>21603.8340401813</v>
+      </c>
+      <c r="C4">
+        <v>68122</v>
+      </c>
       <c r="F4">
-        <f>MIN(Tableau2[Temps])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="e">
+        <f>MIN(Tableau2[Score])</f>
+        <v>15430.3485701798</v>
+      </c>
+      <c r="G4">
         <f>AVERAGE(Tableau2[Score])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="e">
-        <f>AVERAGE(Tableau2[Temps])</f>
-        <v>#DIV/0!</v>
+        <v>18746.474153893385</v>
+      </c>
+      <c r="H4">
+        <f>SUM(Tableau2[Temps])</f>
+        <v>627586</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>18432.964688982502</v>
+      </c>
+      <c r="C5">
+        <v>103869</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>20286.559918964402</v>
+      </c>
+      <c r="C6">
+        <v>104740</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>18288.911491074399</v>
+      </c>
+      <c r="C7">
+        <v>106146</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>18436.226213977901</v>
+      </c>
+      <c r="C8">
+        <v>111798</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>15430.3485701798</v>
+      </c>
+      <c r="C10">
+        <v>132911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>